<commit_message>
Timo toegevoegd aan documentatie
</commit_message>
<xml_diff>
--- a/Documentatie/Planning.xlsx
+++ b/Documentatie/Planning.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TCR School\Project\Project2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Chirpify\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70362ADA-E513-4162-A595-CD1EA17CC225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6348D4-F4AF-42BA-9B92-D7D539F6A805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BA9973BC-ED01-4649-A3BA-F440FF000B7E}"/>
   </bookViews>
@@ -120,9 +120,6 @@
     <t>Planning Project 2 - Chirpify</t>
   </si>
   <si>
-    <t>Teamleden: Tahiru Agbanwa, Ody Chen, Quinten van den Dungen Bille</t>
-  </si>
-  <si>
     <t>Alle benodigde programma's installeren, GitHub Repository aanmaken, Project opzetten, Ontwikkelomgeving opzetten, Planning maken, Definition of Done en Definition of Fun opstellen.</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>29-01-2024 t/m 03-02-2024</t>
+  </si>
+  <si>
+    <t>Teamleden: Tahiru Agbanwa, Ody Chen, Quinten van den Dungen Bille, Timo Korpershoek</t>
   </si>
 </sst>
 </file>
@@ -291,6 +291,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -298,47 +334,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,7 +656,7 @@
   <dimension ref="A1:U20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:D20"/>
+      <selection activeCell="A2" sqref="A2:U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -665,54 +665,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="20"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="8"/>
     </row>
     <row r="2" spans="1:21" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="23"/>
+      <c r="A2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="11"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -753,7 +753,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="5"/>
       <c r="E4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -776,55 +776,55 @@
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="12">
         <v>45254</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="8"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="20"/>
     </row>
     <row r="6" spans="1:21" ht="21" x14ac:dyDescent="0.4">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="14"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="17"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -836,7 +836,7 @@
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
       <c r="E7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -859,30 +859,30 @@
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="12">
         <v>45261</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="8"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="20"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -894,7 +894,7 @@
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
       <c r="E9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -917,55 +917,55 @@
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="12">
         <v>45268</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="8"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="20"/>
     </row>
     <row r="11" spans="1:21" ht="21" x14ac:dyDescent="0.4">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="14"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="17"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -977,7 +977,7 @@
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -1006,7 +1006,7 @@
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
       <c r="E13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -1027,55 +1027,55 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="6" t="s">
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="7"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="8"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="20"/>
     </row>
     <row r="15" spans="1:21" ht="21" x14ac:dyDescent="0.4">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="14"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="16"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="17"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -1087,7 +1087,7 @@
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
       <c r="E16" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1115,25 +1115,25 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16"/>
-      <c r="T17" s="16"/>
-      <c r="U17" s="17"/>
+      <c r="E17" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="23"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -1168,42 +1168,42 @@
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="12">
         <v>45316</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="6" t="s">
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="8"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="20"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="5"/>
       <c r="E20" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -1224,11 +1224,22 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A2:U2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:U3"/>
+    <mergeCell ref="E18:U18"/>
+    <mergeCell ref="E20:U20"/>
+    <mergeCell ref="E10:U10"/>
+    <mergeCell ref="E19:U19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E13:U13"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A15:U15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E16:U16"/>
+    <mergeCell ref="E14:U14"/>
+    <mergeCell ref="E17:U17"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="A11:U11"/>
     <mergeCell ref="B9:D9"/>
@@ -1238,27 +1249,16 @@
     <mergeCell ref="E8:U8"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
-    <mergeCell ref="A15:U15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E16:U16"/>
-    <mergeCell ref="E14:U14"/>
-    <mergeCell ref="E17:U17"/>
-    <mergeCell ref="E4:U4"/>
     <mergeCell ref="E7:U7"/>
     <mergeCell ref="E5:U5"/>
     <mergeCell ref="E9:U9"/>
     <mergeCell ref="E12:U12"/>
-    <mergeCell ref="E18:U18"/>
-    <mergeCell ref="E20:U20"/>
-    <mergeCell ref="E10:U10"/>
-    <mergeCell ref="E19:U19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E13:U13"/>
-    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A2:U2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:U3"/>
+    <mergeCell ref="E4:U4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>